<commit_message>
going through the debriefings
</commit_message>
<xml_diff>
--- a/results/analysis/waveData/batch_0_wave_1/wave_debriefing.xlsx
+++ b/results/analysis/waveData/batch_0_wave_1/wave_debriefing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\concept_gen_analysis\results\analysis\waveData\batch_0_wave_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8BA178-317A-447D-BBA2-475E25F203BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A258A99A-04BC-4CB0-A1DB-4F75D42BFED1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="122" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,15 +663,18 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="20.7109375" style="2"/>
+    <col min="1" max="16384" width="20.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +727,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -774,7 +777,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -815,7 +818,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -868,7 +871,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -918,7 +921,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -932,7 +935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -973,7 +976,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>